<commit_message>
Bruno: Docs / Fix GMS IA que podia dar freeza com v?rtices isolados
</commit_message>
<xml_diff>
--- a/entrega/Tarefas(ParaEntrega).xlsx
+++ b/entrega/Tarefas(ParaEntrega).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\LaprV\entrega\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>Tarefas</t>
   </si>
@@ -69,9 +74,6 @@
     <t>Picking</t>
   </si>
   <si>
-    <t>Dimensão da rede de um utilizador</t>
-  </si>
-  <si>
     <t>Permitir associar a outros utlizadores</t>
   </si>
   <si>
@@ -108,9 +110,6 @@
     <t>Determinar caminho mais forte entre 2 utilizadores baseado em relações (familia/amigo/conhecido)</t>
   </si>
   <si>
-    <t>Estrutura rede da social</t>
-  </si>
-  <si>
     <t>Mini-mapa</t>
   </si>
   <si>
@@ -196,6 +195,15 @@
   </si>
   <si>
     <t>Tags de relação entre utilizadores</t>
+  </si>
+  <si>
+    <t>Conexão IA</t>
+  </si>
+  <si>
+    <t>Estrutura rede da social (C/ ligação BD)</t>
+  </si>
+  <si>
+    <t>Texturas</t>
   </si>
 </sst>
 </file>
@@ -450,6 +458,246 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -606,246 +854,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1642,7 +1650,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:F19" headerRowCount="0" totalsRowShown="0" headerRowDxfId="84" dataDxfId="82" headerRowBorderDxfId="83" tableBorderDxfId="81" totalsRowBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:F20" headerRowCount="0" totalsRowShown="0" headerRowDxfId="84" dataDxfId="82" headerRowBorderDxfId="83" tableBorderDxfId="81" totalsRowBorderDxfId="80">
   <tableColumns count="6">
     <tableColumn id="1" name="Column1" headerRowDxfId="79" dataDxfId="78"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="77" dataDxfId="76"/>
@@ -1656,7 +1664,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A23:F34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66" tableBorderDxfId="64" totalsRowBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A24:F36" headerRowCount="0" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66" tableBorderDxfId="64" totalsRowBorderDxfId="63">
   <tableColumns count="6">
     <tableColumn id="1" name="Column1" headerRowDxfId="62" dataDxfId="61"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="60" dataDxfId="59"/>
@@ -1670,7 +1678,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A38:F48" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A40:F50" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <tableColumns count="6">
     <tableColumn id="1" name="Column1" headerRowDxfId="45" dataDxfId="44"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="43" dataDxfId="42"/>
@@ -1684,7 +1692,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A52:F55" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A54:F57" headerRowCount="0" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Column1" headerRowDxfId="28" dataDxfId="27"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="26" dataDxfId="25"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="24" dataDxfId="23"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="22" dataDxfId="21"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="20" dataDxfId="19"/>
+    <tableColumn id="6" name="Column6" headerRowDxfId="18" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A61:F63" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <tableColumns count="6">
     <tableColumn id="1" name="Column1" headerRowDxfId="11" dataDxfId="10"/>
     <tableColumn id="2" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
@@ -1692,20 +1714,6 @@
     <tableColumn id="4" name="Column4" headerRowDxfId="5" dataDxfId="4"/>
     <tableColumn id="5" name="Column5" headerRowDxfId="3" dataDxfId="2"/>
     <tableColumn id="6" name="Column6" headerRowDxfId="1" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A59:F61" headerRowCount="0" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <tableColumns count="6">
-    <tableColumn id="1" name="Column1" headerRowDxfId="28" dataDxfId="27"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="26" dataDxfId="25"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="24" dataDxfId="23"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="22" dataDxfId="21"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="20" dataDxfId="19"/>
-    <tableColumn id="6" name="Column6" headerRowDxfId="18" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1966,7 +1974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1974,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,61 +2036,61 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2092,77 +2100,77 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2174,10 +2182,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
@@ -2188,63 +2196,69 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="A20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
@@ -2255,33 +2269,29 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2293,7 +2303,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2305,11 +2315,9 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="4"/>
@@ -2319,9 +2327,11 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="4"/>
@@ -2331,60 +2341,53 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="4"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="4"/>
       <c r="J31" s="3"/>
@@ -2398,51 +2401,57 @@
         <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="10"/>
+      <c r="B33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="A35" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -2450,12 +2459,16 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="A36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="10"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -2463,14 +2476,12 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2478,19 +2489,12 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -2498,21 +2502,14 @@
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="A39" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -2521,18 +2518,18 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="E40" s="2"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -2541,16 +2538,16 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="3"/>
@@ -2563,15 +2560,15 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="E42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="4"/>
       <c r="G42" s="5"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -2582,17 +2579,17 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>44</v>
+      <c r="A43" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="3"/>
@@ -2603,64 +2600,62 @@
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
     </row>
-    <row r="44" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G44" s="16"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="3"/>
@@ -2672,16 +2667,18 @@
       <c r="N46" s="5"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
+      <c r="A47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G47" s="5"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -2691,100 +2688,98 @@
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-    </row>
-    <row r="49" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-    </row>
-    <row r="50" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+    </row>
+    <row r="50" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+    </row>
+    <row r="51" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" s="10"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -2795,18 +2790,18 @@
       <c r="N53" s="5"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>44</v>
-      </c>
+      <c r="A54" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" s="10"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -2818,15 +2813,15 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B55" s="6"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="E55" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="5"/>
@@ -2839,12 +2834,18 @@
       <c r="N55" s="5"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="A56" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2855,12 +2856,18 @@
       <c r="N56" s="5"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+      <c r="A57" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" s="10"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2871,14 +2878,12 @@
       <c r="N57" s="5"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
@@ -2889,67 +2894,101 @@
       <c r="N58" s="5"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="5"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="B61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>